<commit_message>
schimbari de la lab2
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -73,6 +73,31 @@
     <author>Author</author>
   </authors>
   <commentList>
+    <comment ref="N5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Author:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">fill with DONE or n/a after regression testing
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H18" authorId="0" shapeId="0">
       <text>
         <r>
@@ -83,7 +108,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t xml:space="preserve">Author:
+</t>
         </r>
         <r>
           <rPr>
@@ -92,12 +118,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
-fill with DONE or n/a after re-testing</t>
+          <t xml:space="preserve">fill with DONE or n/a after regression testing
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0" shapeId="0">
+    <comment ref="L18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="111">
   <si>
     <t>VVSS, Info Romana, 2023-2024</t>
   </si>
@@ -191,9 +217,6 @@
   </si>
   <si>
     <t xml:space="preserve">1. La proiectarea TCs se consideră o metodă care poate avea următoarea semnătură: </t>
-  </si>
-  <si>
-    <t>addMovie(String title, String director, int year, List&lt;String&gt; actors, String category, List&lt;String&gt; keywords): void</t>
   </si>
   <si>
     <t>2. Metoda este definită la nivelul repository, service sau ui.</t>
@@ -399,9 +422,6 @@
     <t>Debugging</t>
   </si>
   <si>
-    <t>Re-testing</t>
-  </si>
-  <si>
     <t>Regression Testing</t>
   </si>
   <si>
@@ -530,9 +550,6 @@
   </si>
   <si>
     <t>Cash</t>
-  </si>
-  <si>
-    <t>row added to file</t>
   </si>
   <si>
     <t>Card</t>
@@ -580,8 +597,68 @@
     </r>
   </si>
   <si>
+    <t>table is int in [1,10]</t>
+  </si>
+  <si>
+    <t>amount is double  &gt; 0</t>
+  </si>
+  <si>
+    <t>01. table=2</t>
+  </si>
+  <si>
+    <t>02. table=1</t>
+  </si>
+  <si>
+    <t>03. table=0</t>
+  </si>
+  <si>
+    <t>05. table = 10</t>
+  </si>
+  <si>
+    <t>06. table=11</t>
+  </si>
+  <si>
+    <t>04. table = 9</t>
+  </si>
+  <si>
+    <t>07. amount = 2</t>
+  </si>
+  <si>
+    <t>08. amount=0</t>
+  </si>
+  <si>
+    <t>09. amount=0.01</t>
+  </si>
+  <si>
+    <t>TC1_EC</t>
+  </si>
+  <si>
+    <t>TC2_EC</t>
+  </si>
+  <si>
+    <t>TC4_EC</t>
+  </si>
+  <si>
+    <t>.-3</t>
+  </si>
+  <si>
+    <t>TC2_ECP</t>
+  </si>
+  <si>
+    <t>TC2_BVA</t>
+  </si>
+  <si>
+    <t>TC7_BVA</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>public void addPayment(int table, PaymentType type, double amount) throws Exception</t>
+  </si>
+  <si>
     <r>
-      <t>1,3,5,</t>
+      <t>1,3,5,7</t>
     </r>
     <r>
       <rPr>
@@ -591,84 +668,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>8,11</t>
+      <t>,11</t>
     </r>
   </si>
   <si>
-    <t>table is int in [1,10]</t>
-  </si>
-  <si>
-    <t>amount is double  &gt; 0</t>
-  </si>
-  <si>
-    <t>01. table=2</t>
-  </si>
-  <si>
-    <t>02. table=1</t>
-  </si>
-  <si>
-    <t>03. table=0</t>
-  </si>
-  <si>
-    <t>05. table = 10</t>
-  </si>
-  <si>
-    <t>06. table=11</t>
-  </si>
-  <si>
-    <t>04. table = 9</t>
-  </si>
-  <si>
-    <t>07. amount = 2</t>
-  </si>
-  <si>
-    <t>08. amount=0</t>
-  </si>
-  <si>
-    <t>09. amount=0.01</t>
-  </si>
-  <si>
-    <t>10. amount=-0.01</t>
-  </si>
-  <si>
-    <t>11. amount=1.1</t>
-  </si>
-  <si>
-    <t>12. amount=20.011</t>
-  </si>
-  <si>
-    <t>TC1_EC</t>
-  </si>
-  <si>
-    <t>TC2_EC</t>
-  </si>
-  <si>
-    <t>TC4_EC</t>
-  </si>
-  <si>
-    <t>.-3</t>
-  </si>
-  <si>
-    <t>TC2_ECP</t>
-  </si>
-  <si>
-    <t>TC2_BVA</t>
-  </si>
-  <si>
-    <t>TC7_BVA</t>
-  </si>
-  <si>
-    <t>TC11_BVA</t>
-  </si>
-  <si>
-    <t>yes</t>
+    <t>TC8_BVA</t>
+  </si>
+  <si>
+    <t>Re-Testing</t>
+  </si>
+  <si>
+    <t>exception not thrown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -854,6 +871,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -899,7 +931,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1167,19 +1199,6 @@
       <left style="double">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1255,28 +1274,6 @@
       <top style="double">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1301,7 +1298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1416,12 +1413,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1466,6 +1457,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1512,6 +1506,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1532,17 +1535,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1559,62 +1601,18 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1926,7 +1924,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1939,12 +1937,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="64"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="62"/>
       <c r="H1" s="40" t="s">
         <v>1</v>
       </c>
@@ -1952,11 +1950,11 @@
       <c r="J1" s="40"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="H2" s="65" t="s">
+      <c r="H2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
@@ -1972,7 +1970,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J4" s="2">
         <v>233</v>
@@ -1983,7 +1981,7 @@
         <v>6</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J5" s="2">
         <v>233</v>
@@ -1995,7 +1993,7 @@
         <v>7</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J6" s="2">
         <v>233</v>
@@ -2041,7 +2039,7 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2049,7 +2047,7 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2072,17 +2070,17 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C20" s="36" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -2099,7 +2097,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -2116,21 +2114,21 @@
     </row>
     <row r="24" spans="1:15" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="37"/>
-      <c r="B24" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
-      <c r="L24" s="61"/>
-      <c r="M24" s="61"/>
-      <c r="N24" s="61"/>
+      <c r="B24" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="59"/>
+      <c r="M24" s="59"/>
+      <c r="N24" s="59"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C26" s="39"/>
@@ -2153,8 +2151,8 @@
   </sheetPr>
   <dimension ref="B1:L23"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:L11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2171,217 +2169,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="70" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="72"/>
+      <c r="B3" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="71"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="72" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="G5" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="G5" s="74" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="E6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="G6" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="75" t="s">
+      <c r="H6" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="77" t="s">
+      <c r="I6" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="79" t="s">
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="17" t="s">
         <v>28</v>
-      </c>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="17" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="66" t="s">
-        <v>69</v>
+      <c r="C7" s="65" t="s">
+        <v>67</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="78"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="77"/>
       <c r="I7" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="J7" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>83</v>
-      </c>
       <c r="L7" s="45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="66"/>
+      <c r="C8" s="65"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G8" s="17">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I8" s="2">
         <v>2</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K8" s="2">
         <v>0.01</v>
       </c>
       <c r="L8" s="44" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="67" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>71</v>
+      <c r="C9" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>69</v>
       </c>
       <c r="E9" s="4"/>
       <c r="G9" s="17">
         <v>2</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I9" s="2">
         <v>4</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K9" s="2">
         <v>-0.01</v>
       </c>
       <c r="L9" s="44" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="67"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="50" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" s="52">
+      <c r="E10" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="50">
         <v>3</v>
       </c>
-      <c r="H10" s="53" t="s">
-        <v>89</v>
+      <c r="H10" s="51" t="s">
+        <v>86</v>
       </c>
       <c r="I10" s="27">
         <v>11</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K10" s="27">
         <v>20.010999999999999</v>
       </c>
       <c r="L10" s="46" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="66" t="s">
-        <v>73</v>
+      <c r="C11" s="65" t="s">
+        <v>71</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="G11" s="52">
+      <c r="G11" s="50">
         <v>4</v>
       </c>
       <c r="H11" s="27" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="I11" s="27">
         <v>0</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K11" s="27">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L11" s="46" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="66"/>
+      <c r="C12" s="65"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G12" s="9">
         <v>5</v>
@@ -2396,40 +2394,40 @@
       <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="68" t="s">
-        <v>75</v>
+      <c r="C13" s="67" t="s">
+        <v>73</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E13" s="4"/>
       <c r="G13" s="9">
         <v>6</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L13" s="42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="69"/>
+      <c r="C14" s="68"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G14" s="13">
         <v>7</v>
@@ -2444,18 +2442,18 @@
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="66" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="51" t="s">
-        <v>79</v>
+      <c r="C15" s="65" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="49" t="s">
+        <v>77</v>
       </c>
       <c r="E15" s="4"/>
       <c r="G15" s="13">
         <v>8</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
@@ -2466,10 +2464,10 @@
       <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="51"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="49"/>
       <c r="E16" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="12"/>
@@ -2482,10 +2480,10 @@
       <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="66"/>
+      <c r="C17" s="65"/>
       <c r="D17" s="4"/>
       <c r="E17" s="41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="12"/>
@@ -2498,7 +2496,7 @@
       <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="66"/>
+      <c r="C18" s="65"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="G18" s="13"/>
@@ -2512,7 +2510,7 @@
       <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="66"/>
+      <c r="C19" s="65"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="G19" s="13"/>
@@ -2526,8 +2524,8 @@
       <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="66" t="s">
-        <v>31</v>
+      <c r="C20" s="65" t="s">
+        <v>30</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -2542,16 +2540,16 @@
       <c r="B21" s="4">
         <v>15</v>
       </c>
-      <c r="C21" s="66"/>
+      <c r="C21" s="65"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="81"/>
-      <c r="G23" s="81"/>
+        <v>32</v>
+      </c>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -2582,8 +2580,8 @@
   </sheetPr>
   <dimension ref="B1:N30"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K18" activeCellId="3" sqref="K9:N9 K11:N11 K14:N14 K18:N18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2603,105 +2601,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="72"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="71"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="81" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="3"/>
-      <c r="G5" s="74" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
     </row>
     <row r="6" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="G6" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="G6" s="75" t="s">
+      <c r="H6" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="75" t="s">
+      <c r="I6" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="75" t="s">
+      <c r="J6" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="77" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="90" t="s">
+      <c r="K6" s="82" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="83"/>
+      <c r="M6" s="83"/>
+      <c r="N6" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="47" t="s">
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="67">
+        <v>1</v>
+      </c>
+      <c r="C7" s="85" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="N7" s="45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="68">
-        <v>1</v>
-      </c>
-      <c r="C7" s="83" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="N7" s="45" t="s">
-        <v>30</v>
-      </c>
-    </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="82"/>
-      <c r="C8" s="84"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="86"/>
       <c r="D8" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G8" s="17">
         <v>1</v>
@@ -2710,7 +2708,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="2"/>
@@ -2719,10 +2717,10 @@
       <c r="N8" s="44"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="82"/>
-      <c r="C9" s="84"/>
+      <c r="B9" s="84"/>
+      <c r="C9" s="86"/>
       <c r="D9" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G9" s="13">
         <v>2</v>
@@ -2736,20 +2734,20 @@
         <v>1</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M9" s="2">
         <v>48</v>
       </c>
       <c r="N9" s="44" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="82"/>
-      <c r="C10" s="84"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="86"/>
       <c r="D10" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G10" s="17">
         <v>3</v>
@@ -2758,7 +2756,7 @@
         <v>3</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="27"/>
@@ -2767,10 +2765,10 @@
       <c r="N10" s="46"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="82"/>
-      <c r="C11" s="84"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G11" s="17">
         <v>4</v>
@@ -2784,20 +2782,20 @@
         <v>9</v>
       </c>
       <c r="L11" s="27" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M11" s="27">
         <v>-58</v>
       </c>
       <c r="N11" s="46" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="69"/>
-      <c r="C12" s="85"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="87"/>
       <c r="D12" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G12" s="17">
         <v>5</v>
@@ -2811,24 +2809,24 @@
         <v>10</v>
       </c>
       <c r="L12" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M12" s="27">
         <v>2010</v>
       </c>
       <c r="N12" s="46" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="68">
+      <c r="B13" s="67">
         <v>2</v>
       </c>
-      <c r="C13" s="83" t="s">
-        <v>92</v>
+      <c r="C13" s="85" t="s">
+        <v>88</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G13" s="13">
         <v>6</v>
@@ -2837,7 +2835,7 @@
         <v>6</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J13" s="15"/>
       <c r="K13" s="16"/>
@@ -2846,10 +2844,10 @@
       <c r="N13" s="42"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="82"/>
-      <c r="C14" s="84"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="86"/>
       <c r="D14" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G14" s="17">
         <v>7</v>
@@ -2863,20 +2861,20 @@
         <v>4</v>
       </c>
       <c r="L14" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M14" s="27">
         <v>2</v>
       </c>
       <c r="N14" s="46" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="82"/>
-      <c r="C15" s="84"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="86"/>
       <c r="D15" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G15" s="17">
         <v>8</v>
@@ -2885,7 +2883,7 @@
         <v>8</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="27"/>
@@ -2894,11 +2892,9 @@
       <c r="N15" s="46"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="82"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="B16" s="84"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="2"/>
       <c r="G16" s="17">
         <v>9</v>
       </c>
@@ -2906,7 +2902,7 @@
         <v>9</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="27"/>
@@ -2915,77 +2911,73 @@
       <c r="N16" s="46"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="82"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" s="17">
+      <c r="B17" s="84"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="112">
         <v>10</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="113">
         <v>10</v>
       </c>
-      <c r="I17" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="46"/>
+      <c r="I17" s="114" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" s="114"/>
+      <c r="K17" s="115"/>
+      <c r="L17" s="115"/>
+      <c r="M17" s="115"/>
+      <c r="N17" s="116"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="69"/>
-      <c r="C18" s="85"/>
-      <c r="D18" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G18" s="17">
+      <c r="B18" s="68"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="112">
         <v>11</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="113">
         <v>11</v>
       </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="L18" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="M18" s="27">
+      <c r="I18" s="114"/>
+      <c r="J18" s="114"/>
+      <c r="K18" s="115" t="s">
+        <v>101</v>
+      </c>
+      <c r="L18" s="115" t="s">
+        <v>83</v>
+      </c>
+      <c r="M18" s="115">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N18" s="46" t="s">
-        <v>87</v>
+      <c r="N18" s="116" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="68">
+      <c r="B19" s="67">
         <v>3</v>
       </c>
-      <c r="C19" s="83"/>
+      <c r="C19" s="85"/>
       <c r="D19" s="2"/>
-      <c r="G19" s="17">
+      <c r="G19" s="112">
         <v>12</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="113">
         <v>12</v>
       </c>
-      <c r="I19" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="J19" s="10"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="46"/>
+      <c r="I19" s="114" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="114"/>
+      <c r="K19" s="115"/>
+      <c r="L19" s="115"/>
+      <c r="M19" s="115"/>
+      <c r="N19" s="116"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="82"/>
-      <c r="C20" s="84"/>
+      <c r="B20" s="84"/>
+      <c r="C20" s="86"/>
       <c r="D20" s="2"/>
       <c r="G20" s="17">
         <v>13</v>
@@ -2999,8 +2991,8 @@
       <c r="N20" s="46"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="82"/>
-      <c r="C21" s="84"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="86"/>
       <c r="D21" s="2"/>
       <c r="G21" s="17">
         <v>14</v>
@@ -3014,8 +3006,8 @@
       <c r="N21" s="46"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="82"/>
-      <c r="C22" s="84"/>
+      <c r="B22" s="84"/>
+      <c r="C22" s="86"/>
       <c r="D22" s="2"/>
       <c r="G22" s="17">
         <v>15</v>
@@ -3029,8 +3021,8 @@
       <c r="N22" s="46"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="82"/>
-      <c r="C23" s="84"/>
+      <c r="B23" s="84"/>
+      <c r="C23" s="86"/>
       <c r="D23" s="2"/>
       <c r="G23" s="17">
         <v>16</v>
@@ -3044,8 +3036,8 @@
       <c r="N23" s="46"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="69"/>
-      <c r="C24" s="85"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="87"/>
       <c r="D24" s="2"/>
       <c r="G24" s="17">
         <v>17</v>
@@ -3059,14 +3051,14 @@
       <c r="N24" s="46"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="68">
+      <c r="B25" s="67">
         <v>4</v>
       </c>
-      <c r="C25" s="83" t="s">
-        <v>31</v>
+      <c r="C25" s="85" t="s">
+        <v>30</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G25" s="17">
         <v>18</v>
@@ -3080,54 +3072,58 @@
       <c r="N25" s="46"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B26" s="82"/>
-      <c r="C26" s="84"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="86"/>
       <c r="D26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B27" s="82"/>
-      <c r="C27" s="84"/>
+      <c r="B27" s="84"/>
+      <c r="C27" s="86"/>
       <c r="D27" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="82"/>
-      <c r="C28" s="84"/>
+      <c r="B28" s="84"/>
+      <c r="C28" s="86"/>
       <c r="D28" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" s="81"/>
-      <c r="H28" s="81"/>
-      <c r="I28" s="88"/>
-      <c r="J28" s="88"/>
-      <c r="K28" s="88"/>
-      <c r="L28" s="88"/>
-      <c r="M28" s="88"/>
+        <v>30</v>
+      </c>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="80"/>
+      <c r="J28" s="80"/>
+      <c r="K28" s="80"/>
+      <c r="L28" s="80"/>
+      <c r="M28" s="80"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="82"/>
-      <c r="C29" s="84"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="86"/>
       <c r="D29" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" s="86"/>
-      <c r="J29" s="86"/>
-      <c r="K29" s="86"/>
-      <c r="L29" s="86"/>
-      <c r="M29" s="86"/>
+        <v>30</v>
+      </c>
+      <c r="I29" s="88"/>
+      <c r="J29" s="88"/>
+      <c r="K29" s="88"/>
+      <c r="L29" s="88"/>
+      <c r="M29" s="88"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B30" s="69"/>
-      <c r="C30" s="85"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="87"/>
       <c r="D30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="G28:H28"/>
     <mergeCell ref="I28:M28"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="H6:H7"/>
@@ -3144,10 +3140,6 @@
     <mergeCell ref="C13:C18"/>
     <mergeCell ref="C19:C24"/>
     <mergeCell ref="B19:B24"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="G28:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3160,177 +3152,177 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B1:L21"/>
+  <dimension ref="B1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="12.21875" style="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" style="52" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5546875" customWidth="1"/>
     <col min="9" max="9" width="30.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="62" t="s">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="62"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="111" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="75" t="s">
+      <c r="C4" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="D4" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="100" t="s">
+      <c r="E4" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="77" t="s">
+      <c r="F4" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="107" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="107"/>
+    </row>
+    <row r="5" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="102"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="79" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="92" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="92"/>
-    </row>
-    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="99"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="55" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="I5" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B6" s="18">
         <v>1</v>
       </c>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>49</v>
-      </c>
       <c r="E6" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="56">
+        <v>31</v>
+      </c>
+      <c r="F6" s="54">
         <v>2</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H6" s="2">
         <v>0.01</v>
       </c>
       <c r="I6" s="44" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="8">
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="97"/>
+      <c r="C7" s="100"/>
       <c r="D7" s="24" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="56">
+        <v>31</v>
+      </c>
+      <c r="F7" s="54">
         <v>4</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H7" s="2">
         <v>-0.01</v>
       </c>
       <c r="I7" s="44" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="8">
         <f t="shared" ref="B8:B13" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="97"/>
+      <c r="C8" s="100"/>
       <c r="D8" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="57">
+        <v>31</v>
+      </c>
+      <c r="F8" s="55">
         <v>11</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H8" s="27">
         <v>20.010999999999999</v>
       </c>
       <c r="I8" s="46" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="97"/>
+      <c r="C9" s="100"/>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
@@ -3338,277 +3330,305 @@
       <c r="H9" s="24"/>
       <c r="I9" s="24"/>
       <c r="J9" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="97"/>
+      <c r="C10" s="100"/>
       <c r="D10" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F10" s="56">
+        <v>103</v>
+      </c>
+      <c r="F10" s="54">
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H10" s="2">
         <v>48</v>
       </c>
       <c r="I10" s="44" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="97"/>
+      <c r="C11" s="100"/>
       <c r="D11" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="57">
+        <v>50</v>
+      </c>
+      <c r="F11" s="55">
         <v>9</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H11" s="27">
         <v>-58</v>
       </c>
       <c r="I11" s="46" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="97"/>
+      <c r="C12" s="100"/>
       <c r="D12" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="F12" s="57">
+        <v>104</v>
+      </c>
+      <c r="F12" s="55">
         <v>4</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H12" s="27">
         <v>2</v>
       </c>
       <c r="I12" s="46" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="19">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C13" s="98"/>
+      <c r="C13" s="101"/>
       <c r="D13" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="F13" s="57" t="s">
         <v>108</v>
       </c>
+      <c r="F13" s="55">
+        <v>0</v>
+      </c>
       <c r="G13" s="27" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H13" s="27">
         <v>1.1000000000000001</v>
       </c>
       <c r="I13" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J13" s="19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="22"/>
       <c r="E14" s="21"/>
-      <c r="F14" s="58"/>
+      <c r="F14" s="56"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
       <c r="J14" s="21"/>
     </row>
-    <row r="15" spans="2:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="22"/>
       <c r="E15" s="21"/>
-      <c r="F15" s="59"/>
+      <c r="F15" s="57"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="106" t="s">
+    <row r="17" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="92" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="94"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="107"/>
-      <c r="E17" s="107"/>
-      <c r="F17" s="108"/>
-      <c r="G17" s="30" t="s">
+      <c r="H17" s="92" t="s">
+        <v>109</v>
+      </c>
+      <c r="I17" s="93"/>
+      <c r="J17" s="94"/>
+      <c r="K17" s="95"/>
+      <c r="L17" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="49" t="s">
+      <c r="M17" s="93"/>
+      <c r="N17" s="94"/>
+      <c r="O17" s="95"/>
+    </row>
+    <row r="18" spans="2:15" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="105" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="106" t="s">
+      <c r="D18" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="J17" s="113"/>
-      <c r="K17" s="107"/>
-      <c r="L17" s="108"/>
-    </row>
-    <row r="18" spans="2:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="102" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="103" t="s">
+      <c r="E18" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="104" t="s">
+      <c r="F18" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="104" t="s">
+      <c r="G18" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="105" t="s">
+      <c r="H18" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="111" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="109" t="s">
-        <v>62</v>
-      </c>
-      <c r="I18" s="114" t="s">
-        <v>62</v>
-      </c>
-      <c r="J18" s="104" t="s">
+      <c r="I18" s="90" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" s="90" t="s">
+        <v>56</v>
+      </c>
+      <c r="K18" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="K18" s="104" t="s">
-        <v>58</v>
-      </c>
-      <c r="L18" s="112" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="102"/>
-      <c r="C19" s="103"/>
-      <c r="D19" s="104"/>
-      <c r="E19" s="104"/>
-      <c r="F19" s="105"/>
-      <c r="G19" s="111"/>
-      <c r="H19" s="110"/>
-      <c r="I19" s="115"/>
-      <c r="J19" s="104"/>
-      <c r="K19" s="104"/>
-      <c r="L19" s="112"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L18" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="M18" s="90" t="s">
+        <v>55</v>
+      </c>
+      <c r="N18" s="90" t="s">
+        <v>56</v>
+      </c>
+      <c r="O18" s="91" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B19" s="105"/>
+      <c r="C19" s="106"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="99"/>
+      <c r="H19" s="97"/>
+      <c r="I19" s="90"/>
+      <c r="J19" s="90"/>
+      <c r="K19" s="91"/>
+      <c r="L19" s="97"/>
+      <c r="M19" s="90"/>
+      <c r="N19" s="90"/>
+      <c r="O19" s="91"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="29">
         <v>7</v>
       </c>
       <c r="D20" s="31">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E20" s="31">
-        <v>2</v>
-      </c>
-      <c r="F20" s="60">
+        <v>4</v>
+      </c>
+      <c r="F20" s="58">
         <v>2</v>
       </c>
       <c r="G20" s="35">
         <v>2</v>
       </c>
-      <c r="H20" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="I20" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="J20" s="2">
+      <c r="H20" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="I20" s="2">
+        <v>4</v>
+      </c>
+      <c r="J20" s="31">
+        <v>4</v>
+      </c>
+      <c r="K20" s="32">
         <v>0</v>
       </c>
-      <c r="K20" s="31">
-        <v>7</v>
-      </c>
-      <c r="L20" s="32">
+      <c r="L20" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="M20" s="2">
+        <v>3</v>
+      </c>
+      <c r="N20" s="31">
+        <v>3</v>
+      </c>
+      <c r="O20" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="I21" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="G18:G19"/>
+  <mergeCells count="26">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B3:J3"/>
     <mergeCell ref="C6:C13"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3617,12 +3637,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3770,15 +3787,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B0A340A-7B8D-463A-B976-63A023B5D9BB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3802,10 +3823,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B0A340A-7B8D-463A-B976-63A023B5D9BB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>